<commit_message>
before going to lab
</commit_message>
<xml_diff>
--- a/Control_Ckt.xlsx
+++ b/Control_Ckt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>OPCODE</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>MemtoReg</t>
-  </si>
-  <si>
-    <t>ALUOP</t>
   </si>
   <si>
     <t>MemWrite</t>
@@ -561,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,10 +571,10 @@
     <col min="16" max="16" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -610,9 +607,8 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -650,13 +646,13 @@
         <v>43</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>46</v>
@@ -665,17 +661,14 @@
         <v>48</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="V2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="1"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V2" s="1"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>0</v>
@@ -737,12 +730,9 @@
       <c r="U3" s="1">
         <v>0</v>
       </c>
-      <c r="V3" s="1">
-        <v>0</v>
-      </c>
-      <c r="W3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>0</v>
@@ -804,12 +794,9 @@
       <c r="U4" s="1">
         <v>0</v>
       </c>
-      <c r="V4" s="1">
-        <v>0</v>
-      </c>
-      <c r="W4" s="1"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>0</v>
@@ -863,20 +850,17 @@
         <v>0</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5" s="1">
         <v>0</v>
       </c>
-      <c r="V5" s="1">
-        <v>0</v>
-      </c>
-      <c r="W5" s="1"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>0</v>
@@ -933,17 +917,14 @@
         <v>0</v>
       </c>
       <c r="T6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" s="1">
-        <v>1</v>
-      </c>
-      <c r="V6" s="1">
-        <v>0</v>
-      </c>
-      <c r="W6" s="1"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>0</v>
@@ -1005,12 +986,9 @@
       <c r="U7" s="1">
         <v>0</v>
       </c>
-      <c r="V7" s="1">
-        <v>0</v>
-      </c>
-      <c r="W7" s="1"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>0</v>
@@ -1072,12 +1050,9 @@
       <c r="U8" s="1">
         <v>0</v>
       </c>
-      <c r="V8" s="1">
-        <v>0</v>
-      </c>
-      <c r="W8" s="1"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V8" s="1"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>0</v>
@@ -1139,12 +1114,9 @@
       <c r="U9" s="1">
         <v>0</v>
       </c>
-      <c r="V9" s="1">
-        <v>0</v>
-      </c>
-      <c r="W9" s="1"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V9" s="1"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>1</v>
@@ -1206,12 +1178,9 @@
       <c r="U10" s="1">
         <v>0</v>
       </c>
-      <c r="V10" s="1">
-        <v>0</v>
-      </c>
-      <c r="W10" s="1"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>1</v>
@@ -1273,12 +1242,9 @@
       <c r="U11" s="1">
         <v>0</v>
       </c>
-      <c r="V11" s="1">
-        <v>0</v>
-      </c>
-      <c r="W11" s="1"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V11" s="1"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>1</v>
@@ -1340,12 +1306,9 @@
       <c r="U12" s="1">
         <v>0</v>
       </c>
-      <c r="V12" s="1">
-        <v>0</v>
-      </c>
-      <c r="W12" s="1"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>1</v>
@@ -1401,18 +1364,15 @@
       <c r="S13" s="1">
         <v>0</v>
       </c>
-      <c r="T13" s="1">
-        <v>0</v>
-      </c>
-      <c r="U13" s="1" t="s">
+      <c r="T13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V13" s="1">
-        <v>1</v>
-      </c>
-      <c r="W13" s="1"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="U13" s="1">
+        <v>1</v>
+      </c>
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>1</v>
@@ -1474,12 +1434,9 @@
       <c r="U14" s="1">
         <v>0</v>
       </c>
-      <c r="V14" s="1">
-        <v>0</v>
-      </c>
-      <c r="W14" s="1"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1502,9 +1459,8 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1527,9 +1483,8 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1552,7 +1507,6 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>